<commit_message>
Revert "things being edited"
This reverts commit 1703731a3617179181378f4a5e1cf13bf4579f3f.
</commit_message>
<xml_diff>
--- a/Sprint Backlog.xlsx
+++ b/Sprint Backlog.xlsx
@@ -5,7 +5,7 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\back up of school files\Software Design &amp; Development\SDDGroupProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atm15_000\Documents\GitHub\SDDGroupProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="129">
   <si>
     <t>Sprint Backlog Template:
 - Rollover unclosed user stories from the preivious sprint. 
@@ -401,6 +401,9 @@
     <t>Other ships are able to be played</t>
   </si>
   <si>
+    <t>Enemies take different amounts of daamge or certain weapon types to deal extra damage</t>
+  </si>
+  <si>
     <t>The user is able to learn how to play</t>
   </si>
   <si>
@@ -422,41 +425,17 @@
     <t>the sound is able to be paused or audio level changed</t>
   </si>
   <si>
-    <t>needs to be cleaned up due to introduction of bugs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">done </t>
-  </si>
-  <si>
-    <t>base level bullets are implementd, higher level bullets are not</t>
-  </si>
-  <si>
-    <t>api hooks created for use for weapon and ship classes to damage enemies</t>
-  </si>
-  <si>
-    <t>Enemies take different amounts of damge or certain weapon types to deal extra damage</t>
-  </si>
-  <si>
-    <t>waiting on higher level weapons to be implemented</t>
-  </si>
-  <si>
-    <t>pending all items integrated</t>
-  </si>
-  <si>
-    <t>the pause portion works for the game</t>
-  </si>
-  <si>
-    <t>mouse input works, bugs have been introduced from the additonal ships implemented</t>
-  </si>
-  <si>
-    <t>not able to be implemented this sprint</t>
+    <t>Mechanics work. May polish later and add some animation if time allows</t>
+  </si>
+  <si>
+    <t>base level bullets are implementd, higher level bullets are not. Bullet animation is not implemented</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -529,20 +508,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -959,7 +924,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1285,23 +1250,15 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1636,11 +1593,11 @@
       <c r="G1" s="5"/>
     </row>
     <row r="2" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="89" t="s">
+      <c r="A2" s="90" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="90"/>
-      <c r="C2" s="90"/>
+      <c r="B2" s="91"/>
+      <c r="C2" s="91"/>
     </row>
     <row r="3" spans="1:7" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
@@ -2105,7 +2062,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A30" s="54"/>
       <c r="B30" s="55"/>
       <c r="C30" s="30" t="s">
@@ -2719,10 +2676,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G59"/>
+  <dimension ref="A1:G58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2770,26 +2727,26 @@
       <c r="F3" s="68"/>
       <c r="G3" s="69"/>
     </row>
-    <row r="4" spans="1:7" ht="38.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="91" t="s">
+    <row r="4" spans="1:7" ht="32.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="91" t="s">
+      <c r="B4" s="82" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="91" t="s">
+      <c r="C4" s="82" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="91" t="s">
+      <c r="D4" s="82" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="91" t="s">
+      <c r="E4" s="82" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="91" t="s">
+      <c r="F4" s="82" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="91" t="s">
+      <c r="G4" s="82" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2821,7 +2778,9 @@
       <c r="F6" s="83" t="s">
         <v>75</v>
       </c>
-      <c r="G6" s="83"/>
+      <c r="G6" s="83" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="7" spans="1:7" ht="57" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="84"/>
@@ -2840,7 +2799,7 @@
       </c>
       <c r="G7" s="83"/>
     </row>
-    <row r="8" spans="1:7" ht="57" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="84"/>
       <c r="B8" s="84"/>
       <c r="C8" s="83" t="s">
@@ -2944,16 +2903,12 @@
       <c r="E14" s="84" t="s">
         <v>118</v>
       </c>
-      <c r="F14" s="84" t="s">
-        <v>75</v>
-      </c>
-      <c r="G14" s="84" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="72.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F14" s="84"/>
+      <c r="G14" s="84"/>
+    </row>
+    <row r="15" spans="1:7" ht="39" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="84"/>
-      <c r="B15" s="92" t="s">
+      <c r="B15" s="89" t="s">
         <v>26</v>
       </c>
       <c r="C15" s="84"/>
@@ -2963,12 +2918,8 @@
       <c r="E15" s="83" t="s">
         <v>117</v>
       </c>
-      <c r="F15" s="84" t="s">
-        <v>127</v>
-      </c>
-      <c r="G15" s="84" t="s">
-        <v>126</v>
-      </c>
+      <c r="F15" s="84"/>
+      <c r="G15" s="84"/>
     </row>
     <row r="16" spans="1:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="84"/>
@@ -3002,8 +2953,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="57" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="93"/>
+    <row r="18" spans="1:7" ht="38.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B18" s="83"/>
       <c r="C18" s="86" t="s">
         <v>42</v>
@@ -3015,26 +2965,22 @@
         <v>71</v>
       </c>
       <c r="F18" s="83" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="G18" s="83" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="83"/>
       <c r="B19" s="83"/>
-      <c r="C19" s="93"/>
-      <c r="D19" s="93"/>
-      <c r="E19" s="93"/>
-      <c r="F19" s="93"/>
-      <c r="G19" s="93"/>
+      <c r="E19" s="65"/>
     </row>
     <row r="20" spans="1:7" ht="38.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="85" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="92" t="s">
+      <c r="B20" s="89" t="s">
         <v>111</v>
       </c>
       <c r="C20" s="86"/>
@@ -3042,18 +2988,14 @@
         <v>60</v>
       </c>
       <c r="E20" s="83" t="s">
-        <v>130</v>
-      </c>
-      <c r="F20" s="83" t="s">
-        <v>77</v>
-      </c>
-      <c r="G20" s="83" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>119</v>
+      </c>
+      <c r="F20" s="83"/>
+      <c r="G20" s="83"/>
+    </row>
+    <row r="21" spans="1:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="83"/>
-      <c r="B21" s="92"/>
+      <c r="B21" s="89"/>
       <c r="C21" s="86"/>
       <c r="D21" s="86"/>
       <c r="E21" s="83"/>
@@ -3072,35 +3014,33 @@
         <v>94</v>
       </c>
       <c r="E22" s="87" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F22" s="87" t="s">
-        <v>75</v>
-      </c>
-      <c r="G22" s="87"/>
-    </row>
-    <row r="23" spans="1:7" ht="37.5" thickBot="1" x14ac:dyDescent="0.35">
+        <v>76</v>
+      </c>
+      <c r="G22" s="87" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="87"/>
-      <c r="B23" s="92" t="s">
+      <c r="B23" s="89" t="s">
         <v>109</v>
       </c>
       <c r="C23" s="87"/>
       <c r="D23" s="87" t="s">
         <v>94</v>
       </c>
-      <c r="E23" s="93" t="s">
-        <v>121</v>
-      </c>
-      <c r="F23" s="87" t="s">
-        <v>77</v>
-      </c>
-      <c r="G23" s="87" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="38.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E23" s="65" t="s">
+        <v>122</v>
+      </c>
+      <c r="F23" s="87"/>
+      <c r="G23" s="87"/>
+    </row>
+    <row r="24" spans="1:7" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="87"/>
-      <c r="B24" s="92" t="s">
+      <c r="B24" s="89" t="s">
         <v>110</v>
       </c>
       <c r="C24" s="87"/>
@@ -3108,25 +3048,21 @@
         <v>94</v>
       </c>
       <c r="E24" s="87" t="s">
-        <v>120</v>
-      </c>
-      <c r="F24" s="87" t="s">
-        <v>76</v>
-      </c>
-      <c r="G24" s="87" t="s">
-        <v>133</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="F24" s="87"/>
+      <c r="G24" s="87"/>
     </row>
     <row r="25" spans="1:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="87"/>
-      <c r="B25" s="92"/>
+      <c r="B25" s="89"/>
       <c r="C25" s="87"/>
       <c r="D25" s="87"/>
       <c r="E25" s="87"/>
       <c r="F25" s="87"/>
       <c r="G25" s="87"/>
     </row>
-    <row r="26" spans="1:7" ht="57" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" ht="38.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="87" t="s">
         <v>11</v>
       </c>
@@ -3138,14 +3074,12 @@
         <v>96</v>
       </c>
       <c r="E26" s="87" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F26" s="87" t="s">
         <v>76</v>
       </c>
-      <c r="G26" s="87" t="s">
-        <v>134</v>
-      </c>
+      <c r="G26" s="87"/>
     </row>
     <row r="27" spans="1:7" ht="38.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="87"/>
@@ -3157,7 +3091,7 @@
         <v>96</v>
       </c>
       <c r="E27" s="87" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F27" s="87" t="s">
         <v>77</v>
@@ -3166,54 +3100,33 @@
         <v>102</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="87"/>
-      <c r="B28" s="88"/>
-      <c r="C28" s="87"/>
-      <c r="D28" s="87"/>
-      <c r="E28" s="87"/>
-      <c r="F28" s="87"/>
-      <c r="G28" s="87"/>
-    </row>
-    <row r="29" spans="1:7" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="93" t="s">
+    <row r="28" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A28" s="65" t="s">
         <v>114</v>
       </c>
-      <c r="B29" s="92" t="s">
+      <c r="B28" s="89" t="s">
         <v>112</v>
       </c>
-      <c r="C29" s="93"/>
-      <c r="D29" s="93" t="s">
+      <c r="D28" s="65" t="s">
         <v>115</v>
       </c>
-      <c r="E29" s="93" t="s">
-        <v>124</v>
-      </c>
-      <c r="F29" s="93" t="s">
-        <v>76</v>
-      </c>
-      <c r="G29" s="93" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="93"/>
-      <c r="B30" s="92" t="s">
+      <c r="E28" s="65" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B29" s="89" t="s">
         <v>113</v>
       </c>
-      <c r="C30" s="93"/>
-      <c r="D30" s="93" t="s">
+      <c r="D29" s="65" t="s">
         <v>116</v>
       </c>
-      <c r="E30" s="93" t="s">
-        <v>125</v>
-      </c>
-      <c r="F30" s="93" t="s">
-        <v>76</v>
-      </c>
-      <c r="G30" s="93" t="s">
-        <v>135</v>
-      </c>
+      <c r="E29" s="65" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="E30" s="65"/>
     </row>
     <row r="31" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="E31" s="65"/>
@@ -3257,18 +3170,16 @@
     <row r="44" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="E44" s="65"/>
     </row>
-    <row r="45" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="E45" s="65"/>
-    </row>
-    <row r="46" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="70"/>
-      <c r="B46" s="71"/>
-      <c r="C46" s="72"/>
-      <c r="D46" s="73"/>
-      <c r="E46" s="71"/>
-      <c r="F46" s="73"/>
-      <c r="G46" s="72"/>
-    </row>
+    <row r="45" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="70"/>
+      <c r="B45" s="71"/>
+      <c r="C45" s="72"/>
+      <c r="D45" s="73"/>
+      <c r="E45" s="71"/>
+      <c r="F45" s="73"/>
+      <c r="G45" s="72"/>
+    </row>
+    <row r="46" spans="1:7" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="47" spans="1:7" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="48" spans="1:7" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="49" ht="12.75" x14ac:dyDescent="0.2"/>
@@ -3280,8 +3191,7 @@
     <row r="55" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="56" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="57" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="58" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="59" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="58" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updates to the backlog for the sprint and updated the contribution for michael
</commit_message>
<xml_diff>
--- a/Sprint Backlog.xlsx
+++ b/Sprint Backlog.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="141">
   <si>
     <t>Sprint Backlog Template:
 - Rollover unclosed user stories from the preivious sprint. 
@@ -452,12 +452,27 @@
   <si>
     <t>Sprint 4</t>
   </si>
+  <si>
+    <t>the player is damaged when hit by a enemy shot</t>
+  </si>
+  <si>
+    <t>weapons do differing amounts of damage to the ships</t>
+  </si>
+  <si>
+    <t>all items have over behavior for them</t>
+  </si>
+  <si>
+    <t>audio does play but the volume is not controllable, not mutes</t>
+  </si>
+  <si>
+    <t>different weapons are implemented</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -530,6 +545,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -946,7 +967,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1287,11 +1308,38 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2542,7 +2590,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="38.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="57" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="83"/>
       <c r="B23" s="83"/>
       <c r="C23" s="86" t="s">
@@ -3261,10 +3309,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G49"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3312,290 +3360,274 @@
       <c r="F3" s="68"/>
       <c r="G3" s="69"/>
     </row>
-    <row r="4" spans="1:7" ht="32.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="81" t="s">
+    <row r="4" spans="1:7" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="A4" s="93" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="82" t="s">
+      <c r="B4" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="82" t="s">
+      <c r="C4" s="94" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="82" t="s">
+      <c r="D4" s="94" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="82" t="s">
+      <c r="E4" s="94" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="82" t="s">
+      <c r="F4" s="94" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="82" t="s">
+      <c r="G4" s="94" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="57" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="83" t="s">
+    <row r="5" spans="1:7" ht="56.25" x14ac:dyDescent="0.2">
+      <c r="A5" s="95" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="83"/>
-      <c r="C5" s="83" t="s">
+      <c r="B5" s="95"/>
+      <c r="C5" s="95" t="s">
         <v>55</v>
       </c>
-      <c r="D5" s="83" t="s">
+      <c r="D5" s="95" t="s">
         <v>46</v>
       </c>
-      <c r="E5" s="83" t="s">
+      <c r="E5" s="95" t="s">
         <v>56</v>
       </c>
-      <c r="F5" s="83" t="s">
+      <c r="F5" s="95" t="s">
+        <v>75</v>
+      </c>
+      <c r="G5" s="95" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="37.5" x14ac:dyDescent="0.2">
+      <c r="A6" s="96"/>
+      <c r="B6" s="95" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="95" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="95" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="95" t="s">
+        <v>63</v>
+      </c>
+      <c r="F6" s="95" t="s">
         <v>76</v>
       </c>
-      <c r="G5" s="83" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="38.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="84"/>
-      <c r="B6" s="83" t="s">
-        <v>40</v>
-      </c>
-      <c r="C6" s="83" t="s">
-        <v>40</v>
-      </c>
-      <c r="D6" s="83" t="s">
+      <c r="G6" s="95" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="A7" s="96"/>
+      <c r="B7" s="96"/>
+      <c r="C7" s="95"/>
+      <c r="D7" s="95"/>
+      <c r="E7" s="95"/>
+      <c r="F7" s="95"/>
+      <c r="G7" s="95"/>
+    </row>
+    <row r="8" spans="1:7" ht="56.25" x14ac:dyDescent="0.2">
+      <c r="A8" s="95" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="95" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="95" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="95" t="s">
         <v>49</v>
       </c>
-      <c r="E6" s="83" t="s">
-        <v>63</v>
-      </c>
-      <c r="F6" s="83" t="s">
+      <c r="E8" s="95" t="s">
+        <v>64</v>
+      </c>
+      <c r="F8" s="95" t="s">
         <v>76</v>
       </c>
-      <c r="G6" s="83" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="84"/>
-      <c r="B7" s="84"/>
-      <c r="C7" s="83"/>
-      <c r="D7" s="83"/>
-      <c r="E7" s="83"/>
-      <c r="F7" s="83"/>
-      <c r="G7" s="83"/>
-    </row>
-    <row r="8" spans="1:7" ht="57" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="83" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="83" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="83" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" s="83" t="s">
-        <v>49</v>
-      </c>
-      <c r="E8" s="83" t="s">
-        <v>64</v>
-      </c>
-      <c r="F8" s="83" t="s">
+      <c r="G8" s="95" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="A9" s="96"/>
+      <c r="B9" s="96"/>
+      <c r="C9" s="96"/>
+      <c r="D9" s="96"/>
+      <c r="E9" s="96"/>
+      <c r="F9" s="96"/>
+      <c r="G9" s="96"/>
+    </row>
+    <row r="10" spans="1:7" ht="56.25" x14ac:dyDescent="0.2">
+      <c r="A10" s="95" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="95" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="95" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="95" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" s="95" t="s">
+        <v>70</v>
+      </c>
+      <c r="F10" s="95" t="s">
+        <v>75</v>
+      </c>
+      <c r="G10" s="95" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="95"/>
+      <c r="B11" s="95"/>
+      <c r="C11" s="97"/>
+      <c r="D11" s="97"/>
+      <c r="E11" s="97"/>
+      <c r="F11" s="97"/>
+      <c r="G11" s="97"/>
+    </row>
+    <row r="12" spans="1:7" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A12" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="98" t="s">
+        <v>111</v>
+      </c>
+      <c r="C12" s="99"/>
+      <c r="D12" s="99" t="s">
+        <v>60</v>
+      </c>
+      <c r="E12" s="95" t="s">
+        <v>127</v>
+      </c>
+      <c r="F12" s="95" t="s">
+        <v>75</v>
+      </c>
+      <c r="G12" s="95" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="95"/>
+      <c r="B13" s="98"/>
+      <c r="C13" s="99"/>
+      <c r="D13" s="99"/>
+      <c r="E13" s="95"/>
+      <c r="F13" s="95"/>
+      <c r="G13" s="95"/>
+    </row>
+    <row r="14" spans="1:7" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A14" s="100"/>
+      <c r="B14" s="98" t="s">
+        <v>109</v>
+      </c>
+      <c r="C14" s="100"/>
+      <c r="D14" s="100" t="s">
+        <v>94</v>
+      </c>
+      <c r="E14" s="97" t="s">
+        <v>119</v>
+      </c>
+      <c r="F14" s="100" t="s">
+        <v>75</v>
+      </c>
+      <c r="G14" s="100" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A15" s="100"/>
+      <c r="B15" s="98"/>
+      <c r="C15" s="100"/>
+      <c r="D15" s="100"/>
+      <c r="E15" s="100"/>
+      <c r="F15" s="100"/>
+      <c r="G15" s="100"/>
+    </row>
+    <row r="16" spans="1:7" ht="56.25" x14ac:dyDescent="0.3">
+      <c r="A16" s="100" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="101" t="s">
+        <v>131</v>
+      </c>
+      <c r="C16" s="100"/>
+      <c r="D16" s="100" t="s">
+        <v>96</v>
+      </c>
+      <c r="E16" s="100" t="s">
+        <v>120</v>
+      </c>
+      <c r="F16" s="100" t="s">
         <v>76</v>
       </c>
-      <c r="G8" s="83" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="84"/>
-      <c r="B9" s="84"/>
-      <c r="C9" s="84"/>
-      <c r="D9" s="84"/>
-      <c r="E9" s="84"/>
-      <c r="F9" s="84"/>
-      <c r="G9" s="84"/>
-    </row>
-    <row r="10" spans="1:7" ht="57" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="83" t="s">
-        <v>34</v>
-      </c>
-      <c r="B10" s="83" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" s="83" t="s">
-        <v>41</v>
-      </c>
-      <c r="D10" s="83" t="s">
-        <v>50</v>
-      </c>
-      <c r="E10" s="83" t="s">
-        <v>70</v>
-      </c>
-      <c r="F10" s="83" t="s">
+      <c r="G16" s="100" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A17" s="100"/>
+      <c r="B17" s="101" t="s">
+        <v>95</v>
+      </c>
+      <c r="C17" s="100"/>
+      <c r="D17" s="100" t="s">
+        <v>96</v>
+      </c>
+      <c r="E17" s="100" t="s">
+        <v>121</v>
+      </c>
+      <c r="F17" s="100" t="s">
+        <v>77</v>
+      </c>
+      <c r="G17" s="100" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="A18" s="97"/>
+      <c r="B18" s="98"/>
+      <c r="C18" s="97"/>
+      <c r="D18" s="97"/>
+      <c r="E18" s="97"/>
+      <c r="F18" s="97"/>
+      <c r="G18" s="97"/>
+    </row>
+    <row r="19" spans="1:7" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A19" s="100" t="s">
+        <v>113</v>
+      </c>
+      <c r="B19" s="101" t="s">
+        <v>112</v>
+      </c>
+      <c r="C19" s="100"/>
+      <c r="D19" s="100" t="s">
+        <v>114</v>
+      </c>
+      <c r="E19" s="100" t="s">
+        <v>122</v>
+      </c>
+      <c r="F19" s="100" t="s">
         <v>76</v>
       </c>
-      <c r="G10" s="83" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="83"/>
-      <c r="B11" s="83"/>
-      <c r="C11" s="90"/>
-      <c r="D11" s="90"/>
-      <c r="E11" s="90"/>
-      <c r="F11" s="90"/>
-      <c r="G11" s="90"/>
-    </row>
-    <row r="12" spans="1:7" ht="38.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="85" t="s">
-        <v>37</v>
-      </c>
-      <c r="B12" s="89" t="s">
-        <v>111</v>
-      </c>
-      <c r="C12" s="86"/>
-      <c r="D12" s="86" t="s">
-        <v>60</v>
-      </c>
-      <c r="E12" s="83" t="s">
-        <v>127</v>
-      </c>
-      <c r="F12" s="83" t="s">
-        <v>77</v>
-      </c>
-      <c r="G12" s="83" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="83"/>
-      <c r="B13" s="89"/>
-      <c r="C13" s="86"/>
-      <c r="D13" s="86"/>
-      <c r="E13" s="83"/>
-      <c r="F13" s="83"/>
-      <c r="G13" s="83"/>
-    </row>
-    <row r="14" spans="1:7" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="87"/>
-      <c r="B14" s="89" t="s">
-        <v>109</v>
-      </c>
-      <c r="C14" s="87"/>
-      <c r="D14" s="87" t="s">
-        <v>94</v>
-      </c>
-      <c r="E14" s="90" t="s">
-        <v>119</v>
-      </c>
-      <c r="F14" s="87" t="s">
-        <v>77</v>
-      </c>
-      <c r="G14" s="87" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="38.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="87"/>
-      <c r="B15" s="89" t="s">
-        <v>110</v>
-      </c>
-      <c r="C15" s="87"/>
-      <c r="D15" s="87" t="s">
-        <v>94</v>
-      </c>
-      <c r="E15" s="87" t="s">
-        <v>118</v>
-      </c>
-      <c r="F15" s="87" t="s">
-        <v>76</v>
-      </c>
-      <c r="G15" s="87" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="87"/>
-      <c r="B16" s="89"/>
-      <c r="C16" s="87"/>
-      <c r="D16" s="87"/>
-      <c r="E16" s="87"/>
-      <c r="F16" s="87"/>
-      <c r="G16" s="87"/>
-    </row>
-    <row r="17" spans="1:7" ht="57" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="87" t="s">
-        <v>11</v>
-      </c>
-      <c r="B17" s="88" t="s">
-        <v>131</v>
-      </c>
-      <c r="C17" s="87"/>
-      <c r="D17" s="87" t="s">
-        <v>96</v>
-      </c>
-      <c r="E17" s="87" t="s">
-        <v>120</v>
-      </c>
-      <c r="F17" s="87" t="s">
-        <v>76</v>
-      </c>
-      <c r="G17" s="87" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="38.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="87"/>
-      <c r="B18" s="88" t="s">
-        <v>95</v>
-      </c>
-      <c r="C18" s="87"/>
-      <c r="D18" s="87" t="s">
-        <v>96</v>
-      </c>
-      <c r="E18" s="87" t="s">
-        <v>121</v>
-      </c>
-      <c r="F18" s="87" t="s">
-        <v>77</v>
-      </c>
-      <c r="G18" s="87" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A19" s="90"/>
-      <c r="B19" s="89"/>
-      <c r="C19" s="90"/>
-      <c r="D19" s="90"/>
-      <c r="E19" s="90"/>
-      <c r="F19" s="90"/>
-      <c r="G19" s="90"/>
-    </row>
-    <row r="20" spans="1:7" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="A20" s="93" t="s">
-        <v>113</v>
-      </c>
-      <c r="B20" s="94" t="s">
-        <v>112</v>
-      </c>
-      <c r="C20" s="93"/>
-      <c r="D20" s="93" t="s">
-        <v>114</v>
-      </c>
-      <c r="E20" s="93" t="s">
-        <v>122</v>
-      </c>
-      <c r="F20" s="93" t="s">
-        <v>76</v>
-      </c>
-      <c r="G20" s="93" t="s">
-        <v>133</v>
-      </c>
+      <c r="G19" s="100" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="E20" s="65"/>
     </row>
     <row r="21" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="E21" s="65"/>
@@ -3639,18 +3671,16 @@
     <row r="34" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="E34" s="65"/>
     </row>
-    <row r="35" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="E35" s="65"/>
-    </row>
-    <row r="36" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="70"/>
-      <c r="B36" s="71"/>
-      <c r="C36" s="72"/>
-      <c r="D36" s="73"/>
-      <c r="E36" s="71"/>
-      <c r="F36" s="73"/>
-      <c r="G36" s="72"/>
-    </row>
+    <row r="35" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="70"/>
+      <c r="B35" s="71"/>
+      <c r="C35" s="72"/>
+      <c r="D35" s="73"/>
+      <c r="E35" s="71"/>
+      <c r="F35" s="73"/>
+      <c r="G35" s="72"/>
+    </row>
+    <row r="36" spans="1:7" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="37" spans="1:7" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="38" spans="1:7" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="39" spans="1:7" ht="12.75" x14ac:dyDescent="0.2"/>
@@ -3662,8 +3692,7 @@
     <row r="45" spans="1:7" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="46" spans="1:7" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="47" spans="1:7" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="48" spans="1:7" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="48" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updates for sprint 3, 4, and 5
</commit_message>
<xml_diff>
--- a/Sprint Backlog.xlsx
+++ b/Sprint Backlog.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="144">
   <si>
     <t>Sprint Backlog Template:
 - Rollover unclosed user stories from the preivious sprint. 
@@ -473,6 +473,9 @@
   </si>
   <si>
     <t>As a player, I want to choose to have music and sound effect on or off.</t>
+  </si>
+  <si>
+    <t>introduction of weapons, added new images for use when ship is moving, added temporary invulnerable state and image when damaged</t>
   </si>
 </sst>
 </file>
@@ -2769,8 +2772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2993,7 +2996,7 @@
         <v>116</v>
       </c>
       <c r="F14" s="84" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G14" s="84" t="s">
         <v>124</v>
@@ -3322,7 +3325,7 @@
   <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:G19"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3636,11 +3639,29 @@
         <v>139</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E20" s="65"/>
     </row>
-    <row r="21" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="E21" s="65"/>
+    <row r="21" spans="1:7" ht="94.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="84" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="84" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="84"/>
+      <c r="D21" s="84" t="s">
+        <v>48</v>
+      </c>
+      <c r="E21" s="84" t="s">
+        <v>116</v>
+      </c>
+      <c r="F21" s="84" t="s">
+        <v>76</v>
+      </c>
+      <c r="G21" s="84" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="22" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="E22" s="65"/>
@@ -3714,7 +3735,7 @@
   <dimension ref="A1:G43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3975,10 +3996,22 @@
       </c>
       <c r="E18" s="65"/>
     </row>
-    <row r="19" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="89" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" s="65" t="s">
+        <v>48</v>
+      </c>
       <c r="E19" s="65"/>
     </row>
-    <row r="20" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="38.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="84" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" s="65" t="s">
+        <v>48</v>
+      </c>
       <c r="E20" s="65"/>
     </row>
     <row r="21" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">

</xml_diff>